<commit_message>
Updates to names of data sets for ease of metadata description
</commit_message>
<xml_diff>
--- a/READ ME - Green Valley Lake Project Metadata.xlsx
+++ b/READ ME - Green Valley Lake Project Metadata.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Box Sync\Butts_Scripts\GV Grazing\chapter1-plankton-func\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Box Sync\Butts_Scripts\GV Grazing\chapter1-hyper-plankton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E082E-4C02-4252-A4F8-35D611694B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CD04B1-2ADA-41AE-AECE-E90831DFC616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="7260" windowHeight="11385" activeTab="3" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
+    <workbookView xWindow="6195" yWindow="1485" windowWidth="9450" windowHeight="12705" firstSheet="5" activeTab="6" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="zp_dat" sheetId="1" r:id="rId1"/>
-    <sheet name="zp_stoich" sheetId="3" r:id="rId2"/>
-    <sheet name="phy_biomass" sheetId="4" r:id="rId3"/>
-    <sheet name="phy_grouping" sheetId="5" r:id="rId4"/>
+    <sheet name="2019_site4_gv_zoopdata" sheetId="1" r:id="rId1"/>
+    <sheet name="2019_zoop_cnpratios" sheetId="3" r:id="rId2"/>
+    <sheet name="2019_site4_gv_phydata" sheetId="4" r:id="rId3"/>
+    <sheet name="2019_gv_phytoplanktongrouping" sheetId="5" r:id="rId4"/>
+    <sheet name="2019_gv_gald-bodymass" sheetId="6" r:id="rId5"/>
+    <sheet name="2019_gv_gald-length" sheetId="7" r:id="rId6"/>
+    <sheet name="2019_gv_nutrients" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="100">
   <si>
     <t>Column Header</t>
   </si>
@@ -242,12 +245,161 @@
   <si>
     <t xml:space="preserve">genera or phyla of identified phytoplankton </t>
   </si>
+  <si>
+    <t>doy</t>
+  </si>
+  <si>
+    <t>gald</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>greatest axial linear distance of a phytoplankton single-cell or colony</t>
+  </si>
+  <si>
+    <t>micrograms</t>
+  </si>
+  <si>
+    <t>individual zooplankton bodymass derived from length-weight regressions</t>
+  </si>
+  <si>
+    <t>ocular units</t>
+  </si>
+  <si>
+    <t>multiply value by 2.5 to get micrometers</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">individual zooplankton body size </t>
+  </si>
+  <si>
+    <t>micrometers</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>siteID</t>
+  </si>
+  <si>
+    <t>depthID</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>sampleDepth</t>
+  </si>
+  <si>
+    <t>SRP_ugL</t>
+  </si>
+  <si>
+    <t>flagSRP</t>
+  </si>
+  <si>
+    <t>TP_ugL</t>
+  </si>
+  <si>
+    <t>flagTP</t>
+  </si>
+  <si>
+    <t>TN_mgL</t>
+  </si>
+  <si>
+    <t>flagTN</t>
+  </si>
+  <si>
+    <t>NOx_mgL</t>
+  </si>
+  <si>
+    <t>flagNOx</t>
+  </si>
+  <si>
+    <t>microcystin</t>
+  </si>
+  <si>
+    <t>microcystin_flag</t>
+  </si>
+  <si>
+    <t>year in which sample was taken</t>
+  </si>
+  <si>
+    <t>sampling site within the lake</t>
+  </si>
+  <si>
+    <t>sampling depth at sampling site</t>
+  </si>
+  <si>
+    <t>sampling depths at each station</t>
+  </si>
+  <si>
+    <t>soluble reactive phosphorus concentration</t>
+  </si>
+  <si>
+    <t>data quality flag for SRP data</t>
+  </si>
+  <si>
+    <t>data quality flag for TP data</t>
+  </si>
+  <si>
+    <t>data quality flag for TN data</t>
+  </si>
+  <si>
+    <t>a=value below detection limit, value set to zero
+b=data missing</t>
+  </si>
+  <si>
+    <t>total phosphorus concentration</t>
+  </si>
+  <si>
+    <t>total nitorgen concentration</t>
+  </si>
+  <si>
+    <t>milligrams per liter</t>
+  </si>
+  <si>
+    <t>nitrate (NO3) concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data quality flag for nitrate data </t>
+  </si>
+  <si>
+    <t>total microcystin concentration</t>
+  </si>
+  <si>
+    <t>data quality flag for microcystin data</t>
+  </si>
+  <si>
+    <t>a=value below detection limit, value set to zero
+b=data missing
+c=variable not sampled at this depth, surface only</t>
+  </si>
+  <si>
+    <t>project identifier</t>
+  </si>
+  <si>
+    <t>beachMonitoring=
+dnr319=
+GVLmonitoring=
+sediment=</t>
+  </si>
+  <si>
+    <t>1=(41.11678, -94.3951)
+2=(41.11123, -94.3946)
+3=(41.10345, -94.3894)
+4=(41.09832, -94.3839)
+5=(41.10598, -94.3821)
+6=(41.10945, -94.3801)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +421,12 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -297,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -344,11 +502,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -391,6 +575,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -709,7 +917,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31E61FF-26A5-4E7A-9D57-BE78113787A0}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,4 +1422,460 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5D75E8-4164-4E88-AF5A-E955181388DC}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E539F4AE-38A2-48D4-BF58-CDF6217464EC}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7164A4-592E-4EC6-8349-F11C513D2A76}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" s="15" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" s="15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" s="15" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" s="15" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to code and selection of datasets for ease of Metadata reporting
</commit_message>
<xml_diff>
--- a/READ ME - Green Valley Lake Project Metadata.xlsx
+++ b/READ ME - Green Valley Lake Project Metadata.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Box Sync\Butts_Scripts\GV Grazing\chapter1-hyper-plankton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Box\Butts_Scripts\GV Grazing\chapter1-hyper-plankton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CD04B1-2ADA-41AE-AECE-E90831DFC616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427C1508-3C6B-4824-AE05-6CFFCDC2D6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="1485" windowWidth="9450" windowHeight="12705" firstSheet="5" activeTab="6" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="9" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="2019_site4_gv_zoopdata" sheetId="1" r:id="rId1"/>
-    <sheet name="2019_zoop_cnpratios" sheetId="3" r:id="rId2"/>
-    <sheet name="2019_site4_gv_phydata" sheetId="4" r:id="rId3"/>
-    <sheet name="2019_gv_phytoplanktongrouping" sheetId="5" r:id="rId4"/>
-    <sheet name="2019_gv_gald-bodymass" sheetId="6" r:id="rId5"/>
-    <sheet name="2019_gv_gald-length" sheetId="7" r:id="rId6"/>
-    <sheet name="2019_gv_nutrients" sheetId="8" r:id="rId7"/>
+    <sheet name="2019_gv_nutrients" sheetId="8" r:id="rId1"/>
+    <sheet name="2019_highfrequency_gv_EXO3" sheetId="9" r:id="rId2"/>
+    <sheet name="2019_site4_gv_zoopdata" sheetId="1" r:id="rId3"/>
+    <sheet name="2019_site4_gv_zooplog" sheetId="10" r:id="rId4"/>
+    <sheet name="2019_zoop_cnpratios" sheetId="3" r:id="rId5"/>
+    <sheet name="2019_site4_gv_phydata" sheetId="4" r:id="rId6"/>
+    <sheet name="2019_gv_phytoplanktongrouping" sheetId="5" r:id="rId7"/>
+    <sheet name="2019_gv_gald-bodymass" sheetId="6" r:id="rId8"/>
+    <sheet name="2019_gv_gald-length" sheetId="11" r:id="rId9"/>
+    <sheet name="Hebert_extract_N" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="180">
   <si>
     <t>Column Header</t>
   </si>
@@ -270,15 +273,6 @@
     <t>multiply value by 2.5 to get micrometers</t>
   </si>
   <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">individual zooplankton body size </t>
-  </si>
-  <si>
-    <t>micrometers</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -381,25 +375,325 @@
     <t>project identifier</t>
   </si>
   <si>
-    <t>beachMonitoring=
-dnr319=
-GVLmonitoring=
-sediment=</t>
-  </si>
-  <si>
-    <t>1=(41.11678, -94.3951)
-2=(41.11123, -94.3946)
-3=(41.10345, -94.3894)
-4=(41.09832, -94.3839)
-5=(41.10598, -94.3821)
-6=(41.10945, -94.3801)</t>
+    <t>GVLmonitoring=Water Quality collected for the Iowa Department of Natural Resources Ambient Lakes Monitoring program (https://programs.iowadnr.gov/aquia/) combined with data collected for this project</t>
+  </si>
+  <si>
+    <t>See table 1 above - sampling locations</t>
+  </si>
+  <si>
+    <t>See table 2 above - sampling locations</t>
+  </si>
+  <si>
+    <r>
+      <t>Sonde Data:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> high_frequency_EXO3_gvl_2019.csv</t>
+    </r>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>doyfrac</t>
+  </si>
+  <si>
+    <t>Fraction of the day of year, based on time of day</t>
+  </si>
+  <si>
+    <t>Decimal day of year</t>
+  </si>
+  <si>
+    <t>Day of year</t>
+  </si>
+  <si>
+    <t>timefrac</t>
+  </si>
+  <si>
+    <t>Fraction of a day</t>
+  </si>
+  <si>
+    <t>Values 0-1</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>Site of the sensor deployment (Site 4)</t>
+  </si>
+  <si>
+    <t>chl_rfu</t>
+  </si>
+  <si>
+    <t>Chlorophyll a</t>
+  </si>
+  <si>
+    <t>Raw fluorescence units</t>
+  </si>
+  <si>
+    <t>Total algae probe for YSI EXO3</t>
+  </si>
+  <si>
+    <t>chl</t>
+  </si>
+  <si>
+    <t>Chlorophyll a concentration</t>
+  </si>
+  <si>
+    <r>
+      <t>micrograms per liter (μg L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>Conductivity</t>
+  </si>
+  <si>
+    <t>Micro Siemens per centimeter</t>
+  </si>
+  <si>
+    <t>Temp/conductivity probe on YSI EXO3</t>
+  </si>
+  <si>
+    <t>nLF cond</t>
+  </si>
+  <si>
+    <t>odo_sat</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen saturation</t>
+  </si>
+  <si>
+    <t>Percent saturation</t>
+  </si>
+  <si>
+    <t>Optical dissolved oxygen probe, YSI EXO3</t>
+  </si>
+  <si>
+    <t>odo_satlocal</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen saturation corrected for local pressure</t>
+  </si>
+  <si>
+    <t>odo</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen concentration</t>
+  </si>
+  <si>
+    <r>
+      <t>Milligrams per liter (mg L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>salinity</t>
+  </si>
+  <si>
+    <t>Salinity</t>
+  </si>
+  <si>
+    <t>Practical salinity unity</t>
+  </si>
+  <si>
+    <t>spcond</t>
+  </si>
+  <si>
+    <t>Specific Conductance</t>
+  </si>
+  <si>
+    <t>pc_rfu</t>
+  </si>
+  <si>
+    <t>Phycocyanin</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>Phycocyanin concentration</t>
+  </si>
+  <si>
+    <t>tds</t>
+  </si>
+  <si>
+    <t>Total dissolved solids</t>
+  </si>
+  <si>
+    <t>Milligrams per liter</t>
+  </si>
+  <si>
+    <t>wiper</t>
+  </si>
+  <si>
+    <t>Position of the sensor wiper during the measurement</t>
+  </si>
+  <si>
+    <t>ph</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>(na)</t>
+  </si>
+  <si>
+    <t>Ag/AgCl probe on YSI EXO3</t>
+  </si>
+  <si>
+    <t>ph_mv</t>
+  </si>
+  <si>
+    <t>pH electrical signal</t>
+  </si>
+  <si>
+    <t>Millivolts</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>Water temperature</t>
+  </si>
+  <si>
+    <t>Celsius</t>
+  </si>
+  <si>
+    <t>battery</t>
+  </si>
+  <si>
+    <t>Battery voltage</t>
+  </si>
+  <si>
+    <t>Volts</t>
+  </si>
+  <si>
+    <t>cablepower</t>
+  </si>
+  <si>
+    <t>Cable power voltage</t>
+  </si>
+  <si>
+    <t>lake</t>
+  </si>
+  <si>
+    <t>SAMPLEVOLUME</t>
+  </si>
+  <si>
+    <t>VOLUMECOUNTED</t>
+  </si>
+  <si>
+    <t>TOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volume of zooplankton sample </t>
+  </si>
+  <si>
+    <t xml:space="preserve">volume of subsamples counted </t>
+  </si>
+  <si>
+    <t>milliliters</t>
+  </si>
+  <si>
+    <t>meters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depth of zooplankton </t>
+  </si>
+  <si>
+    <t>A19041162; G19041150
+A= Ambient Lakes Monitoring Program
+G=Green Valley Surface Water Sampling for this project
+19=Year (2019)
+041=Lake ID (Green Valley Lake) 
+162 = Julian Day of Year</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>milligrams</t>
+  </si>
+  <si>
+    <t>nmol N-NH4 ind-1 h-1</t>
+  </si>
+  <si>
+    <t>the natural log of zooplankton dry mass extracted from figure 3A in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer</t>
+  </si>
+  <si>
+    <t>the natural log of ammonia excretion extracted from figure 3A in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>individual zooplankton body size</t>
+  </si>
+  <si>
+    <t>micrometers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,8 +722,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,8 +790,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -528,11 +876,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,11 +1003,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,6 +1051,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2600325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1E107D6-CC3B-4744-B8E1-008003E2A6A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="942976"/>
+          <a:ext cx="4467225" cy="1347362"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3200400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1094667</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>122170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{890B1370-6AB2-406D-BF80-B8EB515326D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5067300" y="971550"/>
+          <a:ext cx="4466517" cy="1246120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -913,6 +1442,692 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7164A4-592E-4EC6-8349-F11C513D2A76}">
+  <dimension ref="A12:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" s="15" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:5" s="15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="26"/>
+    </row>
+    <row r="23" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" s="15" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="1:5" s="15" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D28:E28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E539F4AE-38A2-48D4-BF58-CDF6217464EC}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D7595E-59F0-401E-978D-98E0D375B902}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1285FC8B-8258-43B8-B530-641EA7A60E69}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -920,17 +2135,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
     <col min="4" max="4" width="42" style="13" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,7 +2162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -962,7 +2177,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -977,7 +2192,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -992,7 +2207,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -1009,7 +2224,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +2239,7 @@
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1039,7 +2254,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +2269,7 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -1074,7 +2289,140 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24A93E3-9BC7-46E3-AC2A-D7858A013BE8}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="31"/>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B075BB-A8E3-4173-82F7-16AC0836EFAA}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1082,17 +2430,17 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="42" style="13" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +2457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
@@ -1126,7 +2474,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1141,7 +2489,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
@@ -1158,7 +2506,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +2523,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
@@ -1197,7 +2545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AA0F63-620F-4ECD-B3FE-F6BA17E4BD50}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1205,17 +2553,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="42" style="13" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +2580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -1249,7 +2597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1266,7 +2614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>41</v>
       </c>
@@ -1281,7 +2629,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +2646,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>42</v>
       </c>
@@ -1313,7 +2661,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>43</v>
       </c>
@@ -1326,7 +2674,7 @@
       <c r="D7" s="10"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>44</v>
       </c>
@@ -1349,7 +2697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31E61FF-26A5-4E7A-9D57-BE78113787A0}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1357,17 +2705,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="42" style="13" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +2732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
@@ -1401,7 +2749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1424,7 +2772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5D75E8-4164-4E88-AF5A-E955181388DC}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1432,17 +2780,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
     <col min="4" max="4" width="42" style="13" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +2807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -1474,7 +2822,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -1491,7 +2839,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>56</v>
       </c>
@@ -1511,25 +2859,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E539F4AE-38A2-48D4-BF58-CDF6217464EC}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74466E62-2160-4DC1-A8DE-3AAFF2C56188}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
     <col min="4" max="4" width="42" style="13" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +2894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -1561,7 +2909,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -1578,304 +2926,22 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>64</v>
+        <v>179</v>
       </c>
       <c r="E4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7164A4-592E-4EC6-8349-F11C513D2A76}">
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="42" style="13" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" s="15" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:5" s="15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" s="15" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" s="15" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="22"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Edits to metadata document
</commit_message>
<xml_diff>
--- a/READ ME - Green Valley Lake Project Metadata.xlsx
+++ b/READ ME - Green Valley Lake Project Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Box\Butts_Scripts\GV Grazing\chapter1-hyper-plankton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427C1508-3C6B-4824-AE05-6CFFCDC2D6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522EC650-42D5-4583-9E33-01A355A0729D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="9" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
+    <workbookView xWindow="-32670" yWindow="1275" windowWidth="21600" windowHeight="12675" firstSheet="11" activeTab="13" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
   </bookViews>
   <sheets>
     <sheet name="2019_gv_nutrients" sheetId="8" r:id="rId1"/>
@@ -23,6 +23,12 @@
     <sheet name="2019_gv_gald-bodymass" sheetId="6" r:id="rId8"/>
     <sheet name="2019_gv_gald-length" sheetId="11" r:id="rId9"/>
     <sheet name="Hebert_extract_N" sheetId="7" r:id="rId10"/>
+    <sheet name="Hebert_extract_N_FW" sheetId="12" r:id="rId11"/>
+    <sheet name="Hebert_extract_P" sheetId="13" r:id="rId12"/>
+    <sheet name="Hebert_extract_P_FW" sheetId="14" r:id="rId13"/>
+    <sheet name="Historical_ALM" sheetId="15" r:id="rId14"/>
+    <sheet name="Historic Plankton Data" sheetId="16" r:id="rId15"/>
+    <sheet name="zp_historical" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -43,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="188">
   <si>
     <t>Column Header</t>
   </si>
@@ -688,12 +694,36 @@
   <si>
     <t>micrometers</t>
   </si>
+  <si>
+    <t xml:space="preserve">the natural log of zooplankton dry mass extracted from figure 3A in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer. Data represent only data points from freshwater data sources. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the natural log of ammonia excretion extracted from figure 3A in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer. Data represent only data points from freshwater data sources. </t>
+  </si>
+  <si>
+    <t>the natural log of zooplankton dry mass extracted from figure 3B in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer</t>
+  </si>
+  <si>
+    <t>the natural log of phosphorus extracted from figure 3B in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer</t>
+  </si>
+  <si>
+    <t>nmol P-PO4^3- ind-1 h-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the natural log of zooplankton dry mass extracted from figure 3B in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer. Data represent only data points from freshwater data sources. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the natural log of phosphorus extracted from figure 3B in Hebert et al. 2016 (https://doi.org/10.1890/15-1084.1) using WebPlotDigitizer. Data represent only data points from freshwater data sources. </t>
+  </si>
+  <si>
+    <t>https://programs.iowadnr.gov/aquia/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,6 +793,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -938,10 +976,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1036,8 +1075,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1446,7 +1492,7 @@
   <dimension ref="A12:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A12" sqref="A12:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E539F4AE-38A2-48D4-BF58-CDF6217464EC}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1792,6 +1838,294 @@
       <c r="E3" s="6"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52753957-ACC8-4096-81C6-1EBB2369FFA1}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752C5DA0-7934-4174-9E71-FFBB0144D5A0}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59B1E57-10C7-468D-956D-D242BB2DB672}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="42" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7C4074-A7E4-434E-99EC-8E5D7CAD32BE}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="47.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FF703F79-E282-4693-BC59-F4BFE888B284}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11111FBD-1159-4B21-B049-284EE4CF0AD7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED20257-BD1E-4428-8B35-570C3F432BC4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updating metadata and making sure the code works with streamlining the datasets to reduce the in-code cleaning of datasets
</commit_message>
<xml_diff>
--- a/READ ME - Green Valley Lake Project Metadata.xlsx
+++ b/READ ME - Green Valley Lake Project Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Box\Butts_Scripts\GV Grazing\chapter1-hyper-plankton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522EC650-42D5-4583-9E33-01A355A0729D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AFDBEB-E0B7-4D05-86A0-A074D8D4FEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32670" yWindow="1275" windowWidth="21600" windowHeight="12675" firstSheet="11" activeTab="13" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="14" xr2:uid="{736DE429-7D8B-4D3A-9C01-AAA66EA461EC}"/>
   </bookViews>
   <sheets>
     <sheet name="2019_gv_nutrients" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="Historic Plankton Data" sheetId="16" r:id="rId15"/>
     <sheet name="zp_historical" sheetId="17" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1075,10 +1075,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1777,7 +1777,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1847,7 +1847,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2056,7 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7C4074-A7E4-434E-99EC-8E5D7CAD32BE}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -2087,13 +2087,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2110,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11111FBD-1159-4B21-B049-284EE4CF0AD7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -2135,7 +2135,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D24"/>
+      <selection activeCell="A19" sqref="A19:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2466,7 +2466,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2760,7 +2760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B075BB-A8E3-4173-82F7-16AC0836EFAA}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2883,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AA0F63-620F-4ECD-B3FE-F6BA17E4BD50}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3111,7 +3111,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>